<commit_message>
Buzzer and pathfinding implemented -- Buzzer untested
Co-authored-by: keybo! <p14n0f0rt3@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/STM32L051-Sample-Codes/Servo_PWM/TestCode.xlsx
+++ b/STM32L051-Sample-Codes/Servo_PWM/TestCode.xlsx
@@ -5449,8 +5449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1EA8E3E-9528-48B1-B505-5A91794B9FF7}">
   <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F35" zoomScale="202" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>